<commit_message>
Progression script insertion donnees
</commit_message>
<xml_diff>
--- a/persistance_des_données/mettre_en_place_une_base_de_donnees/exercice_stagiaires/stagiaireAfpa.xlsx
+++ b/persistance_des_données/mettre_en_place_une_base_de_donnees/exercice_stagiaires/stagiaireAfpa.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="stagiaireafpa" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,13 +11,16 @@
     <sheet name="Hebergements" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Groupes" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Formations" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Matieres" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Constitutions" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Animations" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>nomStagiaire</t>
   </si>
@@ -346,7 +349,19 @@
     <t>28-30-87-90</t>
   </si>
   <si>
+    <t>idFormateur</t>
+  </si>
+  <si>
     <t>idGroupe</t>
+  </si>
+  <si>
+    <t>idMatiere</t>
+  </si>
+  <si>
+    <t>idFormation</t>
+  </si>
+  <si>
+    <t>matieres</t>
   </si>
 </sst>
 </file>
@@ -662,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -878,6 +893,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -923,7 +956,7 @@
     <xf fontId="15" fillId="0" borderId="8" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
     <xf fontId="16" fillId="32" borderId="9" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="15" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="15" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -937,6 +970,10 @@
     <xf fontId="15" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -2392,16 +2429,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col bestFit="1" min="1" max="1" width="11.421875"/>
     <col bestFit="1" min="4" max="4" width="83.140625"/>
   </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="4"/>
     </row>
     <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
@@ -2414,6 +2458,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
@@ -2426,6 +2473,9 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>45</v>
       </c>
@@ -2438,6 +2488,9 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
@@ -2572,13 +2625,13 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -2692,6 +2745,382 @@
     <row r="12" ht="14.25">
       <c r="A12" s="8" t="s">
         <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" min="3" max="3" width="49.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"INSERT INTO Matieres (nomMatiere) VALUES ("""&amp;B2&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Matieres (nomMatiere) VALUES ("Sport");</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"INSERT INTO Matieres (nomMatiere) VALUES ("""&amp;B3&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Matieres (nomMatiere) VALUES ("Français");</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"INSERT INTO Matieres (nomMatiere) VALUES ("""&amp;B4&amp;""");"</f>
+        <v xml:space="preserve">INSERT INTO Matieres (nomMatiere) VALUES ("Math");</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="9.8515625"/>
+    <col bestFit="1" min="4" max="4" width="11.28125"/>
+    <col bestFit="1" min="5" max="5" width="9.8515625"/>
+    <col bestFit="1" min="7" max="7" width="56.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <f>VLOOKUP(B10,$A$2:$B$4,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"INSERT INTO constitutions (idMatiere, idFormation) VALUES ("&amp;D2&amp;","&amp;F2&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO constitutions (idMatiere, idFormation) VALUES (1,1);</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <f>VLOOKUP(B11,$A$2:$B$4,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f>"INSERT INTO constitutions (idMatiere, idFormation) VALUES ("&amp;D3&amp;","&amp;F3&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO constitutions (idMatiere, idFormation) VALUES (2,3);</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="14">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4">
+        <f>VLOOKUP(B12,$A$2:$B$4,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <f>"INSERT INTO constitutions (idMatiere, idFormation) VALUES ("&amp;D4&amp;","&amp;F4&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO constitutions (idMatiere, idFormation) VALUES (3,2);</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5">
+        <f>VLOOKUP(B13,$A$2:$B$4,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" t="str">
+        <f>"INSERT INTO constitutions (idMatiere, idFormation) VALUES ("&amp;D5&amp;","&amp;F5&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO constitutions (idMatiere, idFormation) VALUES (4,2);</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <f>VLOOKUP(B14,$A$2:$B$4,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f>"INSERT INTO constitutions (idMatiere, idFormation) VALUES ("&amp;D6&amp;","&amp;F6&amp;");"</f>
+        <v xml:space="preserve">INSERT INTO constitutions (idMatiere, idFormation) VALUES (5,3);</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="11.421875"/>
+    <col bestFit="1" min="2" max="2" width="12.28125"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>